<commit_message>
solved eqn for weight and true prob from recency and sample size
</commit_message>
<xml_diff>
--- a/data/stat probs/jonathan isaac stat probs - condition.xlsx
+++ b/data/stat probs/jonathan isaac stat probs - condition.xlsx
@@ -33,10 +33,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="den 2023 full" sheetId="24" state="visible" r:id="rId24"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nyk 2023 regular" sheetId="25" state="visible" r:id="rId25"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nyk 2023 full" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cha 2023 regular" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cha 2023 full" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sun 2023 regular" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sun 2023 full" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="tue 2023 regular" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="tue 2023 full" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cha 2023 regular" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cha 2023 full" sheetId="30" state="visible" r:id="rId30"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="min 2023 regular" sheetId="31" state="visible" r:id="rId31"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="min 2023 full" sheetId="32" state="visible" r:id="rId32"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4 after 2023 regular" sheetId="33" state="visible" r:id="rId33"/>
@@ -533,28 +533,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -951,28 +951,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -1369,28 +1369,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -1787,28 +1787,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -2205,16 +2205,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -2223,10 +2223,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -2463,16 +2463,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -2481,10 +2481,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -2727,10 +2727,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -2953,10 +2953,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -3173,28 +3173,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -3495,28 +3495,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -3817,16 +3817,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -4043,28 +4043,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -4461,16 +4461,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -4687,28 +4687,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -5105,28 +5105,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -5523,22 +5523,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -5717,22 +5717,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -5911,22 +5911,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -6169,22 +6169,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -6364,7 +6364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6427,22 +6427,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -6471,10 +6471,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -6523,10 +6523,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
@@ -6555,10 +6555,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E6" t="n">
         <v>100</v>
@@ -6587,10 +6587,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7" t="n">
         <v>100</v>
@@ -6608,70 +6608,6 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="n">
-        <v>100</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>100</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>100</v>
-      </c>
-      <c r="E9" t="n">
-        <v>100</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>100</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
         <v>100</v>
       </c>
     </row>
@@ -6686,7 +6622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6749,22 +6685,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -6793,10 +6729,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -6845,10 +6781,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
@@ -6877,10 +6813,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E6" t="n">
         <v>100</v>
@@ -6909,10 +6845,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7" t="n">
         <v>100</v>
@@ -6930,70 +6866,6 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="n">
-        <v>100</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>100</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>100</v>
-      </c>
-      <c r="E9" t="n">
-        <v>100</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>100</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
         <v>100</v>
       </c>
     </row>
@@ -7071,16 +6943,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -7393,28 +7265,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -7811,16 +7683,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -8133,16 +8005,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -8519,16 +8391,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -8905,16 +8777,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -9291,16 +9163,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -9677,16 +9549,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -9871,16 +9743,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -10065,16 +9937,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -10259,16 +10131,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -10453,16 +10325,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -10471,10 +10343,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -10711,28 +10583,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -11129,16 +11001,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -11147,10 +11019,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -11387,28 +11259,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -11645,28 +11517,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -11903,28 +11775,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -12161,28 +12033,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -12419,28 +12291,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -12837,28 +12709,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -13255,16 +13127,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -13641,16 +13513,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -14027,28 +13899,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -14445,28 +14317,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -14863,28 +14735,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">

</xml_diff>